<commit_message>
added more support for FPGA comm
</commit_message>
<xml_diff>
--- a/Sweep_Tables_Examples.xlsx
+++ b/Sweep_Tables_Examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\Master Year 2\Master Thesis\JULIET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F941E17-1793-45C0-BB35-EE185972494D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E79A312-D112-49B9-A1F0-F21B0941BB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4272" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I251" sqref="I251"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,7 +411,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -424,7 +424,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -437,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -463,7 +463,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -476,7 +476,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -489,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -502,7 +502,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -515,7 +515,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -528,7 +528,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -541,7 +541,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -554,7 +554,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -567,7 +567,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -580,7 +580,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -593,7 +593,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -619,7 +619,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -632,7 +632,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -645,7 +645,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -658,7 +658,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -671,7 +671,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -684,7 +684,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -697,7 +697,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -710,7 +710,7 @@
         <v>46</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -723,7 +723,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -736,7 +736,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -749,7 +749,7 @@
         <v>52</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -762,7 +762,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -775,7 +775,7 @@
         <v>56</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -788,7 +788,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -801,7 +801,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -814,7 +814,7 @@
         <v>62</v>
       </c>
       <c r="B33" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -827,7 +827,7 @@
         <v>64</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -840,7 +840,7 @@
         <v>66</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -853,7 +853,7 @@
         <v>68</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -866,7 +866,7 @@
         <v>70</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -879,7 +879,7 @@
         <v>72</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -892,7 +892,7 @@
         <v>74</v>
       </c>
       <c r="B39" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -905,7 +905,7 @@
         <v>76</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -918,7 +918,7 @@
         <v>78</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -931,7 +931,7 @@
         <v>80</v>
       </c>
       <c r="B42" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -944,7 +944,7 @@
         <v>82</v>
       </c>
       <c r="B43" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -957,7 +957,7 @@
         <v>84</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -970,7 +970,7 @@
         <v>86</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -983,7 +983,7 @@
         <v>88</v>
       </c>
       <c r="B46" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -996,7 +996,7 @@
         <v>90</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1009,7 +1009,7 @@
         <v>92</v>
       </c>
       <c r="B48" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1022,7 +1022,7 @@
         <v>94</v>
       </c>
       <c r="B49" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1035,7 +1035,7 @@
         <v>96</v>
       </c>
       <c r="B50" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1048,7 +1048,7 @@
         <v>98</v>
       </c>
       <c r="B51" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>

</xml_diff>